<commit_message>
Add 2-factor full results & analysis
</commit_message>
<xml_diff>
--- a/jupyter/cifar10-full.xlsx
+++ b/jupyter/cifar10-full.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\abe\fltk-testbed\jupyter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C894C96-A8C3-4EC7-A540-51B8EF8CC588}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AAEE96F-12FE-413C-902D-3FEF2C890227}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -423,7 +423,7 @@
   <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -445,6 +445,9 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>48.26</v>
+      </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
@@ -453,6 +456,9 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>48.26</v>
+      </c>
       <c r="B3" t="s">
         <v>3</v>
       </c>
@@ -461,6 +467,9 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>48.26</v>
+      </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -469,6 +478,9 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>50.13</v>
+      </c>
       <c r="B5" t="s">
         <v>3</v>
       </c>
@@ -477,6 +489,9 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>50.13</v>
+      </c>
       <c r="B6" t="s">
         <v>3</v>
       </c>
@@ -485,6 +500,9 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>50.13</v>
+      </c>
       <c r="B7" t="s">
         <v>3</v>
       </c>
@@ -493,6 +511,9 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>47.72</v>
+      </c>
       <c r="B8" t="s">
         <v>3</v>
       </c>
@@ -501,6 +522,9 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>47.72</v>
+      </c>
       <c r="B9" t="s">
         <v>3</v>
       </c>
@@ -509,6 +533,9 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>47.72</v>
+      </c>
       <c r="B10" t="s">
         <v>3</v>
       </c>
@@ -517,6 +544,9 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>42.66</v>
+      </c>
       <c r="B11" t="s">
         <v>3</v>
       </c>
@@ -525,6 +555,9 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>42.66</v>
+      </c>
       <c r="B12" t="s">
         <v>3</v>
       </c>
@@ -533,6 +566,9 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>42.66</v>
+      </c>
       <c r="B13" t="s">
         <v>3</v>
       </c>
@@ -541,6 +577,9 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>48.26</v>
+      </c>
       <c r="B14" t="s">
         <v>8</v>
       </c>
@@ -549,6 +588,9 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>48.26</v>
+      </c>
       <c r="B15" t="s">
         <v>8</v>
       </c>
@@ -557,6 +599,9 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>48.26</v>
+      </c>
       <c r="B16" t="s">
         <v>8</v>
       </c>
@@ -564,7 +609,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>50.13</v>
+      </c>
       <c r="B17" t="s">
         <v>8</v>
       </c>
@@ -572,7 +620,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>50.13</v>
+      </c>
       <c r="B18" t="s">
         <v>8</v>
       </c>
@@ -580,7 +631,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>50.13</v>
+      </c>
       <c r="B19" t="s">
         <v>8</v>
       </c>
@@ -588,7 +642,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>47.72</v>
+      </c>
       <c r="B20" t="s">
         <v>8</v>
       </c>
@@ -596,7 +653,10 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>47.72</v>
+      </c>
       <c r="B21" t="s">
         <v>8</v>
       </c>
@@ -604,7 +664,10 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>47.72</v>
+      </c>
       <c r="B22" t="s">
         <v>8</v>
       </c>
@@ -612,7 +675,10 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>42.66</v>
+      </c>
       <c r="B23" t="s">
         <v>8</v>
       </c>
@@ -620,7 +686,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>42.66</v>
+      </c>
       <c r="B24" t="s">
         <v>8</v>
       </c>
@@ -628,7 +697,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>42.66</v>
+      </c>
       <c r="B25" t="s">
         <v>8</v>
       </c>
@@ -636,7 +708,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>48.26</v>
+      </c>
       <c r="B26" t="s">
         <v>9</v>
       </c>
@@ -644,7 +719,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>48.26</v>
+      </c>
       <c r="B27" t="s">
         <v>9</v>
       </c>
@@ -652,7 +730,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>48.26</v>
+      </c>
       <c r="B28" t="s">
         <v>9</v>
       </c>
@@ -660,7 +741,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>50.13</v>
+      </c>
       <c r="B29" t="s">
         <v>9</v>
       </c>
@@ -668,7 +752,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>50.13</v>
+      </c>
       <c r="B30" t="s">
         <v>9</v>
       </c>
@@ -676,7 +763,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>50.13</v>
+      </c>
       <c r="B31" t="s">
         <v>9</v>
       </c>
@@ -684,7 +774,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>47.72</v>
+      </c>
       <c r="B32" t="s">
         <v>9</v>
       </c>
@@ -692,7 +785,10 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>47.72</v>
+      </c>
       <c r="B33" t="s">
         <v>9</v>
       </c>
@@ -700,7 +796,10 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>47.72</v>
+      </c>
       <c r="B34" t="s">
         <v>9</v>
       </c>
@@ -708,7 +807,10 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>42.66</v>
+      </c>
       <c r="B35" t="s">
         <v>9</v>
       </c>
@@ -716,7 +818,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>42.66</v>
+      </c>
       <c r="B36" t="s">
         <v>9</v>
       </c>
@@ -724,7 +829,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>42.66</v>
+      </c>
       <c r="B37" t="s">
         <v>9</v>
       </c>
@@ -742,7 +850,7 @@
   <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -764,6 +872,9 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>26.15</v>
+      </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
@@ -772,6 +883,9 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>26.65</v>
+      </c>
       <c r="B3" t="s">
         <v>3</v>
       </c>
@@ -780,6 +894,9 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>26.625</v>
+      </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -788,6 +905,9 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>26</v>
+      </c>
       <c r="B5" t="s">
         <v>3</v>
       </c>
@@ -796,6 +916,9 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>23.6</v>
+      </c>
       <c r="B6" t="s">
         <v>3</v>
       </c>
@@ -804,6 +927,9 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>23.274999999999999</v>
+      </c>
       <c r="B7" t="s">
         <v>3</v>
       </c>
@@ -812,6 +938,9 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>25.849</v>
+      </c>
       <c r="B8" t="s">
         <v>3</v>
       </c>
@@ -820,6 +949,9 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>26.6</v>
+      </c>
       <c r="B9" t="s">
         <v>3</v>
       </c>
@@ -828,6 +960,9 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>26.125</v>
+      </c>
       <c r="B10" t="s">
         <v>3</v>
       </c>
@@ -836,6 +971,9 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>22.65</v>
+      </c>
       <c r="B11" t="s">
         <v>3</v>
       </c>
@@ -844,6 +982,9 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>23.625</v>
+      </c>
       <c r="B12" t="s">
         <v>3</v>
       </c>
@@ -852,6 +993,9 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>23.1</v>
+      </c>
       <c r="B13" t="s">
         <v>3</v>
       </c>
@@ -860,6 +1004,9 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>50.674999999999997</v>
+      </c>
       <c r="B14" t="s">
         <v>8</v>
       </c>
@@ -868,6 +1015,9 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>45.9</v>
+      </c>
       <c r="B15" t="s">
         <v>8</v>
       </c>
@@ -876,6 +1026,9 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>46</v>
+      </c>
       <c r="B16" t="s">
         <v>8</v>
       </c>
@@ -883,7 +1036,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>46.55</v>
+      </c>
       <c r="B17" t="s">
         <v>8</v>
       </c>
@@ -891,7 +1047,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>49.875</v>
+      </c>
       <c r="B18" t="s">
         <v>8</v>
       </c>
@@ -899,7 +1058,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>45.3</v>
+      </c>
       <c r="B19" t="s">
         <v>8</v>
       </c>
@@ -907,7 +1069,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>45.024000000000001</v>
+      </c>
       <c r="B20" t="s">
         <v>8</v>
       </c>
@@ -915,7 +1080,10 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>46.024999999999999</v>
+      </c>
       <c r="B21" t="s">
         <v>8</v>
       </c>
@@ -923,7 +1091,10 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>46.225000000000001</v>
+      </c>
       <c r="B22" t="s">
         <v>8</v>
       </c>
@@ -931,7 +1102,10 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>44.575000000000003</v>
+      </c>
       <c r="B23" t="s">
         <v>8</v>
       </c>
@@ -939,7 +1113,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>47.024999999999999</v>
+      </c>
       <c r="B24" t="s">
         <v>8</v>
       </c>
@@ -947,7 +1124,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>48.973999999999997</v>
+      </c>
       <c r="B25" t="s">
         <v>8</v>
       </c>
@@ -955,7 +1135,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>45.3</v>
+      </c>
       <c r="B26" t="s">
         <v>9</v>
       </c>
@@ -963,7 +1146,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>46.5</v>
+      </c>
       <c r="B27" t="s">
         <v>9</v>
       </c>
@@ -971,7 +1157,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>46.674999999999997</v>
+      </c>
       <c r="B28" t="s">
         <v>9</v>
       </c>
@@ -979,7 +1168,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>45.024999999999999</v>
+      </c>
       <c r="B29" t="s">
         <v>9</v>
       </c>
@@ -987,7 +1179,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>45.4</v>
+      </c>
       <c r="B30" t="s">
         <v>9</v>
       </c>
@@ -995,7 +1190,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>50.598999999999997</v>
+      </c>
       <c r="B31" t="s">
         <v>9</v>
       </c>
@@ -1003,7 +1201,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>45.375</v>
+      </c>
       <c r="B32" t="s">
         <v>9</v>
       </c>
@@ -1011,7 +1212,10 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>48.424999999999997</v>
+      </c>
       <c r="B33" t="s">
         <v>9</v>
       </c>
@@ -1019,7 +1223,10 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>49.55</v>
+      </c>
       <c r="B34" t="s">
         <v>9</v>
       </c>
@@ -1027,7 +1234,10 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>44.875</v>
+      </c>
       <c r="B35" t="s">
         <v>9</v>
       </c>
@@ -1035,7 +1245,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>43.774999999999999</v>
+      </c>
       <c r="B36" t="s">
         <v>9</v>
       </c>
@@ -1043,7 +1256,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>42.973999999999997</v>
+      </c>
       <c r="B37" t="s">
         <v>9</v>
       </c>
@@ -1053,6 +1269,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1061,7 +1278,7 @@
   <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1083,6 +1300,9 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>281707.75</v>
+      </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
@@ -1091,6 +1311,9 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>280915.25</v>
+      </c>
       <c r="B3" t="s">
         <v>3</v>
       </c>
@@ -1099,6 +1322,9 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>280129.75</v>
+      </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -1107,6 +1333,9 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>252211.75</v>
+      </c>
       <c r="B5" t="s">
         <v>3</v>
       </c>
@@ -1115,6 +1344,9 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>251046.25</v>
+      </c>
       <c r="B6" t="s">
         <v>3</v>
       </c>
@@ -1123,6 +1355,9 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>254584.25</v>
+      </c>
       <c r="B7" t="s">
         <v>3</v>
       </c>
@@ -1131,6 +1366,9 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>236019.5</v>
+      </c>
       <c r="B8" t="s">
         <v>3</v>
       </c>
@@ -1139,6 +1377,9 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>244353</v>
+      </c>
       <c r="B9" t="s">
         <v>3</v>
       </c>
@@ -1147,6 +1388,9 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>237415</v>
+      </c>
       <c r="B10" t="s">
         <v>3</v>
       </c>
@@ -1155,6 +1399,9 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>255814.25</v>
+      </c>
       <c r="B11" t="s">
         <v>3</v>
       </c>
@@ -1163,6 +1410,9 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>259425.25</v>
+      </c>
       <c r="B12" t="s">
         <v>3</v>
       </c>
@@ -1171,6 +1421,9 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>247506.25</v>
+      </c>
       <c r="B13" t="s">
         <v>3</v>
       </c>
@@ -1179,6 +1432,9 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>136667.25</v>
+      </c>
       <c r="B14" t="s">
         <v>8</v>
       </c>
@@ -1187,6 +1443,9 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>138424.25</v>
+      </c>
       <c r="B15" t="s">
         <v>8</v>
       </c>
@@ -1195,6 +1454,9 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>136837.5</v>
+      </c>
       <c r="B16" t="s">
         <v>8</v>
       </c>
@@ -1202,7 +1464,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>125970.75</v>
+      </c>
       <c r="B17" t="s">
         <v>8</v>
       </c>
@@ -1210,7 +1475,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>126322.75</v>
+      </c>
       <c r="B18" t="s">
         <v>8</v>
       </c>
@@ -1218,7 +1486,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>125614.5</v>
+      </c>
       <c r="B19" t="s">
         <v>8</v>
       </c>
@@ -1226,7 +1497,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>121406</v>
+      </c>
       <c r="B20" t="s">
         <v>8</v>
       </c>
@@ -1234,7 +1508,10 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>122068.5</v>
+      </c>
       <c r="B21" t="s">
         <v>8</v>
       </c>
@@ -1242,7 +1519,10 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>122024.5</v>
+      </c>
       <c r="B22" t="s">
         <v>8</v>
       </c>
@@ -1250,7 +1530,10 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>129412.5</v>
+      </c>
       <c r="B23" t="s">
         <v>8</v>
       </c>
@@ -1258,7 +1541,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>128744.75</v>
+      </c>
       <c r="B24" t="s">
         <v>8</v>
       </c>
@@ -1266,7 +1552,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>135448.5</v>
+      </c>
       <c r="B25" t="s">
         <v>8</v>
       </c>
@@ -1274,7 +1563,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>138225.5</v>
+      </c>
       <c r="B26" t="s">
         <v>9</v>
       </c>
@@ -1282,7 +1574,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>135742.5</v>
+      </c>
       <c r="B27" t="s">
         <v>9</v>
       </c>
@@ -1290,7 +1585,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>134782.25</v>
+      </c>
       <c r="B28" t="s">
         <v>9</v>
       </c>
@@ -1298,7 +1596,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>126399.5</v>
+      </c>
       <c r="B29" t="s">
         <v>9</v>
       </c>
@@ -1306,7 +1607,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>124517.5</v>
+      </c>
       <c r="B30" t="s">
         <v>9</v>
       </c>
@@ -1314,7 +1618,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>124249.25</v>
+      </c>
       <c r="B31" t="s">
         <v>9</v>
       </c>
@@ -1322,7 +1629,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>120889.25</v>
+      </c>
       <c r="B32" t="s">
         <v>9</v>
       </c>
@@ -1330,7 +1640,10 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>121840.5</v>
+      </c>
       <c r="B33" t="s">
         <v>9</v>
       </c>
@@ -1338,7 +1651,10 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>120589.75</v>
+      </c>
       <c r="B34" t="s">
         <v>9</v>
       </c>
@@ -1346,7 +1662,10 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>134018.25</v>
+      </c>
       <c r="B35" t="s">
         <v>9</v>
       </c>
@@ -1354,7 +1673,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>128454.25</v>
+      </c>
       <c r="B36" t="s">
         <v>9</v>
       </c>
@@ -1362,7 +1684,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>139104.25</v>
+      </c>
       <c r="B37" t="s">
         <v>9</v>
       </c>

</xml_diff>